<commit_message>
Anti Player Augmented created, but bugs
</commit_message>
<xml_diff>
--- a/Probability/Analysis.xlsx
+++ b/Probability/Analysis.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Old-New" sheetId="1" r:id="rId1"/>
     <sheet name="Investigation" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Anti" sheetId="6" r:id="rId4"/>
+    <sheet name="Augmented Bugfix" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet3!$H$1:$M$121</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet3!$H$1:$M$121</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="113">
   <si>
     <t>D</t>
   </si>
@@ -195,6 +196,180 @@
   </si>
   <si>
     <t>result</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>A9</t>
+  </si>
+  <si>
+    <t>A11</t>
+  </si>
+  <si>
+    <t>A15</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>A13</t>
+  </si>
+  <si>
+    <t>A14</t>
+  </si>
+  <si>
+    <t>A16</t>
+  </si>
+  <si>
+    <t>A17</t>
+  </si>
+  <si>
+    <t>A18</t>
+  </si>
+  <si>
+    <t>A19</t>
+  </si>
+  <si>
+    <t>Coins</t>
+  </si>
+  <si>
+    <t>Nr</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P0</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>P6</t>
+  </si>
+  <si>
+    <t>P7</t>
+  </si>
+  <si>
+    <t>P8</t>
+  </si>
+  <si>
+    <t>P9</t>
+  </si>
+  <si>
+    <t>P11</t>
+  </si>
+  <si>
+    <t>P15</t>
+  </si>
+  <si>
+    <t>P12</t>
+  </si>
+  <si>
+    <t>P10</t>
+  </si>
+  <si>
+    <t>P13</t>
+  </si>
+  <si>
+    <t>P14</t>
+  </si>
+  <si>
+    <t>P16</t>
+  </si>
+  <si>
+    <t>P17</t>
+  </si>
+  <si>
+    <t>P18</t>
+  </si>
+  <si>
+    <t>P19</t>
+  </si>
+  <si>
+    <t>Probablity</t>
+  </si>
+  <si>
+    <t>DiceP</t>
+  </si>
+  <si>
+    <t>DiceA</t>
+  </si>
+  <si>
+    <t>Scan groups of moves (A6, Ap……A16, A17)</t>
+  </si>
+  <si>
+    <t>Make Coins2 = Coins</t>
+  </si>
+  <si>
+    <t>Calculate sum of (multiplication of all P probabilites * coins2 in the same row) for each A in a group</t>
+  </si>
+  <si>
+    <t>Filter longest (n length) paths where A ends</t>
+  </si>
+  <si>
+    <t>If N&gt;2, replace coins2 with coins2 * A(n) * p(n-1); delete A(n) and p(n-1)</t>
+  </si>
+  <si>
+    <t>While N&gt;1, continue step 3</t>
+  </si>
+  <si>
+    <t>Fill A braincells with -1</t>
+  </si>
+  <si>
+    <t>Verify if any -1 brain cell is left in A</t>
+  </si>
+  <si>
+    <t>Make a copy of A, run normalise, verify if anything is changed</t>
+  </si>
+  <si>
+    <t>Choose the best outcome, fill its A with 1, and replace all other A with 0 in the group (verify if A was -1 before replacement, otherwise - exception)</t>
+  </si>
+  <si>
+    <t>Augmented</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beautify </t>
+  </si>
+  <si>
+    <t>Brutforce</t>
   </si>
 </sst>
 </file>
@@ -220,7 +395,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,18 +410,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -315,11 +496,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -330,8 +552,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,7 +842,7 @@
   <dimension ref="B1:N43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="A1:XFD1048576"/>
+      <selection activeCell="L8" sqref="H8:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1991,10 +2218,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R60"/>
+  <dimension ref="B2:R60"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M6" sqref="M6:M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2043,15 +2270,15 @@
         <v>-1</v>
       </c>
       <c r="D3">
-        <f>IF(O3="",1,O3)</f>
+        <f t="shared" ref="D3:D34" si="0">IF(O3="",1,O3)</f>
         <v>0.7</v>
       </c>
       <c r="E3">
-        <f>IF(P3="",1,P3)</f>
+        <f t="shared" ref="E3:E34" si="1">IF(P3="",1,P3)</f>
         <v>1</v>
       </c>
       <c r="F3">
-        <f>IF(Q3="",1,Q3)</f>
+        <f t="shared" ref="F3:F34" si="2">IF(Q3="",1,Q3)</f>
         <v>1</v>
       </c>
       <c r="G3">
@@ -2074,14 +2301,14 @@
         <v>25</v>
       </c>
       <c r="N3">
-        <f>IF(RIGHT(TRIM(L3),2)="-1",B3,-B3)</f>
+        <f t="shared" ref="N3:N34" si="3">IF(RIGHT(TRIM(L3),2)="-1",B3,-B3)</f>
         <v>-1</v>
       </c>
       <c r="O3">
         <v>0.7</v>
       </c>
       <c r="R3">
-        <f>N3*D3*E3*F3</f>
+        <f t="shared" ref="R3:R34" si="4">N3*D3*E3*F3</f>
         <v>-0.7</v>
       </c>
     </row>
@@ -2090,19 +2317,19 @@
         <v>-1</v>
       </c>
       <c r="D4">
-        <f>IF(O4="",1,O4)</f>
+        <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
       <c r="E4">
-        <f>IF(P4="",1,P4)</f>
+        <f t="shared" si="1"/>
         <v>0.12</v>
       </c>
       <c r="F4">
-        <f>IF(Q4="",1,Q4)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G58" si="0">D4*E4*F4</f>
+        <f t="shared" ref="G4:G58" si="5">D4*E4*F4</f>
         <v>2.3999999999999998E-3</v>
       </c>
       <c r="I4">
@@ -2121,7 +2348,7 @@
         <v>26</v>
       </c>
       <c r="N4">
-        <f>IF(RIGHT(TRIM(L4),2)="-1",B4,-B4)</f>
+        <f t="shared" si="3"/>
         <v>-1</v>
       </c>
       <c r="O4">
@@ -2131,7 +2358,7 @@
         <v>0.12</v>
       </c>
       <c r="R4">
-        <f>N4*D4*E4*F4</f>
+        <f t="shared" si="4"/>
         <v>-2.3999999999999998E-3</v>
       </c>
     </row>
@@ -2140,19 +2367,19 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <f>IF(O5="",1,O5)</f>
+        <f t="shared" si="0"/>
         <v>0.89</v>
       </c>
       <c r="E5">
-        <f>IF(P5="",1,P5)</f>
+        <f t="shared" si="1"/>
         <v>0.12</v>
       </c>
       <c r="F5">
-        <f>IF(Q5="",1,Q5)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.10679999999999999</v>
       </c>
       <c r="I5">
@@ -2171,7 +2398,7 @@
         <v>27</v>
       </c>
       <c r="N5">
-        <f>IF(RIGHT(TRIM(L5),2)="-1",B5,-B5)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O5">
@@ -2181,7 +2408,7 @@
         <v>0.12</v>
       </c>
       <c r="R5">
-        <f>N5*D5*E5*F5</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2190,19 +2417,19 @@
         <v>-1</v>
       </c>
       <c r="D6">
-        <f>IF(O6="",1,O6)</f>
+        <f t="shared" si="0"/>
         <v>0.48</v>
       </c>
       <c r="E6">
-        <f>IF(P6="",1,P6)</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="F6">
-        <f>IF(Q6="",1,Q6)</f>
+        <f t="shared" si="2"/>
         <v>0.26</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1.2480000000000002E-2</v>
       </c>
       <c r="I6">
@@ -2221,7 +2448,7 @@
         <v>28</v>
       </c>
       <c r="N6">
-        <f>IF(RIGHT(TRIM(L6),2)="-1",B6,-B6)</f>
+        <f t="shared" si="3"/>
         <v>-1</v>
       </c>
       <c r="O6">
@@ -2234,7 +2461,7 @@
         <v>0.26</v>
       </c>
       <c r="R6">
-        <f>N6*D6*E6*F6</f>
+        <f t="shared" si="4"/>
         <v>-1.2480000000000002E-2</v>
       </c>
     </row>
@@ -2243,19 +2470,19 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <f>IF(O7="",1,O7)</f>
+        <f t="shared" si="0"/>
         <v>0.52</v>
       </c>
       <c r="E7">
-        <f>IF(P7="",1,P7)</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="F7">
-        <f>IF(Q7="",1,Q7)</f>
+        <f t="shared" si="2"/>
         <v>0.26</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1.3520000000000003E-2</v>
       </c>
       <c r="I7">
@@ -2274,7 +2501,7 @@
         <v>29</v>
       </c>
       <c r="N7">
-        <f>IF(RIGHT(TRIM(L7),2)="-1",B7,-B7)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O7">
@@ -2287,7 +2514,7 @@
         <v>0.26</v>
       </c>
       <c r="R7">
-        <f>N7*D7*E7*F7</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2296,19 +2523,19 @@
         <v>-1</v>
       </c>
       <c r="D8">
-        <f>IF(O8="",1,O8)</f>
+        <f t="shared" si="0"/>
         <v>0.41</v>
       </c>
       <c r="E8">
-        <f>IF(P8="",1,P8)</f>
+        <f t="shared" si="1"/>
         <v>0.77</v>
       </c>
       <c r="F8">
-        <f>IF(Q8="",1,Q8)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.31569999999999998</v>
       </c>
       <c r="I8">
@@ -2327,7 +2554,7 @@
         <v>30</v>
       </c>
       <c r="N8">
-        <f>IF(RIGHT(TRIM(L8),2)="-1",B8,-B8)</f>
+        <f t="shared" si="3"/>
         <v>-1</v>
       </c>
       <c r="O8">
@@ -2337,7 +2564,7 @@
         <v>0.77</v>
       </c>
       <c r="R8">
-        <f>N8*D8*E8*F8</f>
+        <f t="shared" si="4"/>
         <v>-0.31569999999999998</v>
       </c>
     </row>
@@ -2346,19 +2573,19 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <f>IF(O9="",1,O9)</f>
+        <f t="shared" si="0"/>
         <v>0.59</v>
       </c>
       <c r="E9">
-        <f>IF(P9="",1,P9)</f>
+        <f t="shared" si="1"/>
         <v>0.77</v>
       </c>
       <c r="F9">
-        <f>IF(Q9="",1,Q9)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.45429999999999998</v>
       </c>
       <c r="I9">
@@ -2377,7 +2604,7 @@
         <v>31</v>
       </c>
       <c r="N9">
-        <f>IF(RIGHT(TRIM(L9),2)="-1",B9,-B9)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O9">
@@ -2387,7 +2614,7 @@
         <v>0.77</v>
       </c>
       <c r="R9">
-        <f>N9*D9*E9*F9</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2396,21 +2623,21 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <f>IF(O10="",1,O10)</f>
-        <v>0.11</v>
-      </c>
-      <c r="E10">
-        <f>IF(P10="",1,P10)</f>
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <f>IF(Q10="",1,Q10)</f>
-        <v>1</v>
-      </c>
-      <c r="G10">
         <f t="shared" si="0"/>
         <v>0.11</v>
       </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="5"/>
+        <v>0.11</v>
+      </c>
       <c r="I10">
         <v>0</v>
       </c>
@@ -2427,14 +2654,14 @@
         <v>25</v>
       </c>
       <c r="N10">
-        <f>IF(RIGHT(TRIM(L10),2)="-1",B10,-B10)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O10">
         <v>0.11</v>
       </c>
       <c r="R10">
-        <f>N10*D10*E10*F10</f>
+        <f t="shared" si="4"/>
         <v>0.11</v>
       </c>
     </row>
@@ -2443,19 +2670,19 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <f>IF(O11="",1,O11)</f>
+        <f t="shared" si="0"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="E11">
-        <f>IF(P11="",1,P11)</f>
+        <f t="shared" si="1"/>
         <v>0.26</v>
       </c>
       <c r="F11">
-        <f>IF(Q11="",1,Q11)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>3.6400000000000002E-2</v>
       </c>
       <c r="I11">
@@ -2474,7 +2701,7 @@
         <v>26</v>
       </c>
       <c r="N11">
-        <f>IF(RIGHT(TRIM(L11),2)="-1",B11,-B11)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O11">
@@ -2484,7 +2711,7 @@
         <v>0.26</v>
       </c>
       <c r="R11">
-        <f>N11*D11*E11*F11</f>
+        <f t="shared" si="4"/>
         <v>3.6400000000000002E-2</v>
       </c>
     </row>
@@ -2493,19 +2720,19 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <f>IF(O12="",1,O12)</f>
+        <f t="shared" si="0"/>
         <v>0.76</v>
       </c>
       <c r="E12">
-        <f>IF(P12="",1,P12)</f>
+        <f t="shared" si="1"/>
         <v>0.26</v>
       </c>
       <c r="F12">
-        <f>IF(Q12="",1,Q12)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.1976</v>
       </c>
       <c r="I12">
@@ -2524,7 +2751,7 @@
         <v>27</v>
       </c>
       <c r="N12">
-        <f>IF(RIGHT(TRIM(L12),2)="-1",B12,-B12)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O12">
@@ -2534,7 +2761,7 @@
         <v>0.26</v>
       </c>
       <c r="R12">
-        <f>N12*D12*E12*F12</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2543,19 +2770,19 @@
         <v>1</v>
       </c>
       <c r="D13">
-        <f>IF(O13="",1,O13)</f>
+        <f t="shared" si="0"/>
         <v>0.85</v>
       </c>
       <c r="E13">
-        <f>IF(P13="",1,P13)</f>
+        <f t="shared" si="1"/>
         <v>0.09</v>
       </c>
       <c r="F13">
-        <f>IF(Q13="",1,Q13)</f>
+        <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
       <c r="G13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>9.1799999999999989E-3</v>
       </c>
       <c r="I13">
@@ -2574,7 +2801,7 @@
         <v>28</v>
       </c>
       <c r="N13">
-        <f>IF(RIGHT(TRIM(L13),2)="-1",B13,-B13)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O13">
@@ -2587,7 +2814,7 @@
         <v>0.12</v>
       </c>
       <c r="R13">
-        <f>N13*D13*E13*F13</f>
+        <f t="shared" si="4"/>
         <v>9.1799999999999989E-3</v>
       </c>
     </row>
@@ -2596,19 +2823,19 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <f>IF(O14="",1,O14)</f>
+        <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
       <c r="E14">
-        <f>IF(P14="",1,P14)</f>
+        <f t="shared" si="1"/>
         <v>0.09</v>
       </c>
       <c r="F14">
-        <f>IF(Q14="",1,Q14)</f>
+        <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
       <c r="G14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1.6199999999999999E-3</v>
       </c>
       <c r="I14">
@@ -2627,7 +2854,7 @@
         <v>29</v>
       </c>
       <c r="N14">
-        <f>IF(RIGHT(TRIM(L14),2)="-1",B14,-B14)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O14">
@@ -2640,7 +2867,7 @@
         <v>0.12</v>
       </c>
       <c r="R14">
-        <f>N14*D14*E14*F14</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2649,19 +2876,19 @@
         <v>1</v>
       </c>
       <c r="D15">
-        <f>IF(O15="",1,O15)</f>
+        <f t="shared" si="0"/>
         <v>0.16</v>
       </c>
       <c r="E15">
-        <f>IF(P15="",1,P15)</f>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="F15">
-        <f>IF(Q15="",1,Q15)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>6.4000000000000003E-3</v>
       </c>
       <c r="I15">
@@ -2680,7 +2907,7 @@
         <v>30</v>
       </c>
       <c r="N15">
-        <f>IF(RIGHT(TRIM(L15),2)="-1",B15,-B15)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O15">
@@ -2690,7 +2917,7 @@
         <v>0.04</v>
       </c>
       <c r="R15">
-        <f>N15*D15*E15*F15</f>
+        <f t="shared" si="4"/>
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
@@ -2699,19 +2926,19 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <f>IF(O16="",1,O16)</f>
+        <f t="shared" si="0"/>
         <v>0.84</v>
       </c>
       <c r="E16">
-        <f>IF(P16="",1,P16)</f>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="F16">
-        <f>IF(Q16="",1,Q16)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>3.3599999999999998E-2</v>
       </c>
       <c r="I16">
@@ -2730,7 +2957,7 @@
         <v>31</v>
       </c>
       <c r="N16">
-        <f>IF(RIGHT(TRIM(L16),2)="-1",B16,-B16)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O16">
@@ -2740,7 +2967,7 @@
         <v>0.04</v>
       </c>
       <c r="R16">
-        <f>N16*D16*E16*F16</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2749,21 +2976,21 @@
         <v>-1</v>
       </c>
       <c r="D17">
-        <f>IF(O17="",1,O17)</f>
-        <v>0.19</v>
-      </c>
-      <c r="E17">
-        <f>IF(P17="",1,P17)</f>
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <f>IF(Q17="",1,Q17)</f>
-        <v>1</v>
-      </c>
-      <c r="G17">
         <f t="shared" si="0"/>
         <v>0.19</v>
       </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="5"/>
+        <v>0.19</v>
+      </c>
       <c r="I17">
         <v>1</v>
       </c>
@@ -2780,14 +3007,14 @@
         <v>32</v>
       </c>
       <c r="N17">
-        <f>IF(RIGHT(TRIM(L17),2)="-1",B17,-B17)</f>
+        <f t="shared" si="3"/>
         <v>-1</v>
       </c>
       <c r="O17">
         <v>0.19</v>
       </c>
       <c r="R17">
-        <f>N17*D17*E17*F17</f>
+        <f t="shared" si="4"/>
         <v>-0.19</v>
       </c>
     </row>
@@ -2796,19 +3023,19 @@
         <v>-1</v>
       </c>
       <c r="D18">
-        <f>IF(O18="",1,O18)</f>
+        <f t="shared" si="0"/>
         <v>0.68</v>
       </c>
       <c r="E18">
-        <f>IF(P18="",1,P18)</f>
+        <f t="shared" si="1"/>
         <v>0.12</v>
       </c>
       <c r="F18">
-        <f>IF(Q18="",1,Q18)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>8.1600000000000006E-2</v>
       </c>
       <c r="I18">
@@ -2827,7 +3054,7 @@
         <v>33</v>
       </c>
       <c r="N18">
-        <f>IF(RIGHT(TRIM(L18),2)="-1",B18,-B18)</f>
+        <f t="shared" si="3"/>
         <v>-1</v>
       </c>
       <c r="O18">
@@ -2837,7 +3064,7 @@
         <v>0.12</v>
       </c>
       <c r="R18">
-        <f>N18*D18*E18*F18</f>
+        <f t="shared" si="4"/>
         <v>-8.1600000000000006E-2</v>
       </c>
     </row>
@@ -2846,19 +3073,19 @@
         <v>-1</v>
       </c>
       <c r="D19">
-        <f>IF(O19="",1,O19)</f>
+        <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
       <c r="E19">
-        <f>IF(P19="",1,P19)</f>
+        <f t="shared" si="1"/>
         <v>0.12</v>
       </c>
       <c r="F19">
-        <f>IF(Q19="",1,Q19)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>9.5999999999999992E-3</v>
       </c>
       <c r="I19">
@@ -2877,7 +3104,7 @@
         <v>34</v>
       </c>
       <c r="N19">
-        <f>IF(RIGHT(TRIM(L19),2)="-1",B19,-B19)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O19">
@@ -2887,7 +3114,7 @@
         <v>0.12</v>
       </c>
       <c r="R19">
-        <f>N19*D19*E19*F19</f>
+        <f t="shared" si="4"/>
         <v>9.5999999999999992E-3</v>
       </c>
     </row>
@@ -2896,19 +3123,19 @@
         <v>-1</v>
       </c>
       <c r="D20">
-        <f>IF(O20="",1,O20)</f>
+        <f t="shared" si="0"/>
         <v>0.49</v>
       </c>
       <c r="E20">
-        <f>IF(P20="",1,P20)</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="F20">
-        <f>IF(Q20="",1,Q20)</f>
+        <f t="shared" si="2"/>
         <v>0.78</v>
       </c>
       <c r="G20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>3.8220000000000004E-2</v>
       </c>
       <c r="I20">
@@ -2927,7 +3154,7 @@
         <v>35</v>
       </c>
       <c r="N20">
-        <f>IF(RIGHT(TRIM(L20),2)="-1",B20,-B20)</f>
+        <f t="shared" si="3"/>
         <v>-1</v>
       </c>
       <c r="O20">
@@ -2940,7 +3167,7 @@
         <v>0.78</v>
       </c>
       <c r="R20">
-        <f>N20*D20*E20*F20</f>
+        <f t="shared" si="4"/>
         <v>-3.8220000000000004E-2</v>
       </c>
     </row>
@@ -2949,19 +3176,19 @@
         <v>-2</v>
       </c>
       <c r="D21">
-        <f>IF(O21="",1,O21)</f>
+        <f t="shared" si="0"/>
         <v>0.51</v>
       </c>
       <c r="E21">
-        <f>IF(P21="",1,P21)</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="F21">
-        <f>IF(Q21="",1,Q21)</f>
+        <f t="shared" si="2"/>
         <v>0.78</v>
       </c>
       <c r="G21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>3.9780000000000003E-2</v>
       </c>
       <c r="I21">
@@ -2980,7 +3207,7 @@
         <v>36</v>
       </c>
       <c r="N21">
-        <f>IF(RIGHT(TRIM(L21),2)="-1",B21,-B21)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="O21">
@@ -2993,7 +3220,7 @@
         <v>0.78</v>
       </c>
       <c r="R21">
-        <f>N21*D21*E21*F21</f>
+        <f t="shared" si="4"/>
         <v>7.9560000000000006E-2</v>
       </c>
     </row>
@@ -3002,19 +3229,19 @@
         <v>-1</v>
       </c>
       <c r="D22">
-        <f>IF(O22="",1,O22)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E22">
-        <f>IF(P22="",1,P22)</f>
+        <f t="shared" si="1"/>
         <v>0.77</v>
       </c>
       <c r="F22">
-        <f>IF(Q22="",1,Q22)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I22">
@@ -3033,7 +3260,7 @@
         <v>37</v>
       </c>
       <c r="N22">
-        <f>IF(RIGHT(TRIM(L22),2)="-1",B22,-B22)</f>
+        <f t="shared" si="3"/>
         <v>-1</v>
       </c>
       <c r="O22">
@@ -3043,7 +3270,7 @@
         <v>0.77</v>
       </c>
       <c r="R22">
-        <f>N22*D22*E22*F22</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3052,19 +3279,19 @@
         <v>-2</v>
       </c>
       <c r="D23">
-        <f>IF(O23="",1,O23)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E23">
-        <f>IF(P23="",1,P23)</f>
+        <f t="shared" si="1"/>
         <v>0.77</v>
       </c>
       <c r="F23">
-        <f>IF(Q23="",1,Q23)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.77</v>
       </c>
       <c r="I23">
@@ -3083,7 +3310,7 @@
         <v>38</v>
       </c>
       <c r="N23">
-        <f>IF(RIGHT(TRIM(L23),2)="-1",B23,-B23)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="O23">
@@ -3093,7 +3320,7 @@
         <v>0.77</v>
       </c>
       <c r="R23">
-        <f>N23*D23*E23*F23</f>
+        <f t="shared" si="4"/>
         <v>1.54</v>
       </c>
     </row>
@@ -3102,21 +3329,21 @@
         <v>1</v>
       </c>
       <c r="D24">
-        <f>IF(O24="",1,O24)</f>
-        <v>0.11</v>
-      </c>
-      <c r="E24">
-        <f>IF(P24="",1,P24)</f>
-        <v>1</v>
-      </c>
-      <c r="F24">
-        <f>IF(Q24="",1,Q24)</f>
-        <v>1</v>
-      </c>
-      <c r="G24">
         <f t="shared" si="0"/>
         <v>0.11</v>
       </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="5"/>
+        <v>0.11</v>
+      </c>
       <c r="I24">
         <v>1</v>
       </c>
@@ -3133,14 +3360,14 @@
         <v>25</v>
       </c>
       <c r="N24">
-        <f>IF(RIGHT(TRIM(L24),2)="-1",B24,-B24)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O24">
         <v>0.11</v>
       </c>
       <c r="R24">
-        <f>N24*D24*E24*F24</f>
+        <f t="shared" si="4"/>
         <v>0.11</v>
       </c>
     </row>
@@ -3149,19 +3376,19 @@
         <v>1</v>
       </c>
       <c r="D25">
-        <f>IF(O25="",1,O25)</f>
+        <f t="shared" si="0"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="E25">
-        <f>IF(P25="",1,P25)</f>
+        <f t="shared" si="1"/>
         <v>0.78</v>
       </c>
       <c r="F25">
-        <f>IF(Q25="",1,Q25)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.10920000000000002</v>
       </c>
       <c r="I25">
@@ -3180,7 +3407,7 @@
         <v>39</v>
       </c>
       <c r="N25">
-        <f>IF(RIGHT(TRIM(L25),2)="-1",B25,-B25)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O25">
@@ -3190,7 +3417,7 @@
         <v>0.78</v>
       </c>
       <c r="R25">
-        <f>N25*D25*E25*F25</f>
+        <f t="shared" si="4"/>
         <v>0.10920000000000002</v>
       </c>
     </row>
@@ -3199,19 +3426,19 @@
         <v>1</v>
       </c>
       <c r="D26">
-        <f>IF(O26="",1,O26)</f>
+        <f t="shared" si="0"/>
         <v>0.76</v>
       </c>
       <c r="E26">
-        <f>IF(P26="",1,P26)</f>
+        <f t="shared" si="1"/>
         <v>0.78</v>
       </c>
       <c r="F26">
-        <f>IF(Q26="",1,Q26)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.59279999999999999</v>
       </c>
       <c r="I26">
@@ -3230,7 +3457,7 @@
         <v>40</v>
       </c>
       <c r="N26">
-        <f>IF(RIGHT(TRIM(L26),2)="-1",B26,-B26)</f>
+        <f t="shared" si="3"/>
         <v>-1</v>
       </c>
       <c r="O26">
@@ -3240,7 +3467,7 @@
         <v>0.78</v>
       </c>
       <c r="R26">
-        <f>N26*D26*E26*F26</f>
+        <f t="shared" si="4"/>
         <v>-0.59279999999999999</v>
       </c>
     </row>
@@ -3249,19 +3476,19 @@
         <v>1</v>
       </c>
       <c r="D27">
-        <f>IF(O27="",1,O27)</f>
+        <f t="shared" si="0"/>
         <v>0.85</v>
       </c>
       <c r="E27">
-        <f>IF(P27="",1,P27)</f>
+        <f t="shared" si="1"/>
         <v>0.24</v>
       </c>
       <c r="F27">
-        <f>IF(Q27="",1,Q27)</f>
+        <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
       <c r="G27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.4479999999999998E-2</v>
       </c>
       <c r="I27">
@@ -3280,7 +3507,7 @@
         <v>41</v>
       </c>
       <c r="N27">
-        <f>IF(RIGHT(TRIM(L27),2)="-1",B27,-B27)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O27">
@@ -3293,7 +3520,7 @@
         <v>0.12</v>
       </c>
       <c r="R27">
-        <f>N27*D27*E27*F27</f>
+        <f t="shared" si="4"/>
         <v>2.4479999999999998E-2</v>
       </c>
     </row>
@@ -3302,19 +3529,19 @@
         <v>2</v>
       </c>
       <c r="D28">
-        <f>IF(O28="",1,O28)</f>
+        <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
       <c r="E28">
-        <f>IF(P28="",1,P28)</f>
+        <f t="shared" si="1"/>
         <v>0.24</v>
       </c>
       <c r="F28">
-        <f>IF(Q28="",1,Q28)</f>
+        <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
       <c r="G28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>4.3199999999999992E-3</v>
       </c>
       <c r="I28">
@@ -3333,7 +3560,7 @@
         <v>42</v>
       </c>
       <c r="N28">
-        <f>IF(RIGHT(TRIM(L28),2)="-1",B28,-B28)</f>
+        <f t="shared" si="3"/>
         <v>-2</v>
       </c>
       <c r="O28">
@@ -3346,7 +3573,7 @@
         <v>0.12</v>
       </c>
       <c r="R28">
-        <f>N28*D28*E28*F28</f>
+        <f t="shared" si="4"/>
         <v>-8.6399999999999984E-3</v>
       </c>
     </row>
@@ -3355,19 +3582,19 @@
         <v>1</v>
       </c>
       <c r="D29">
-        <f>IF(O29="",1,O29)</f>
+        <f t="shared" si="0"/>
         <v>0.16</v>
       </c>
       <c r="E29">
-        <f>IF(P29="",1,P29)</f>
+        <f t="shared" si="1"/>
         <v>0.03</v>
       </c>
       <c r="F29">
-        <f>IF(Q29="",1,Q29)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="I29">
@@ -3386,7 +3613,7 @@
         <v>43</v>
       </c>
       <c r="N29">
-        <f>IF(RIGHT(TRIM(L29),2)="-1",B29,-B29)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O29">
@@ -3396,7 +3623,7 @@
         <v>0.03</v>
       </c>
       <c r="R29">
-        <f>N29*D29*E29*F29</f>
+        <f t="shared" si="4"/>
         <v>4.7999999999999996E-3</v>
       </c>
     </row>
@@ -3405,19 +3632,19 @@
         <v>2</v>
       </c>
       <c r="D30">
-        <f>IF(O30="",1,O30)</f>
+        <f t="shared" si="0"/>
         <v>0.84</v>
       </c>
       <c r="E30">
-        <f>IF(P30="",1,P30)</f>
+        <f t="shared" si="1"/>
         <v>0.03</v>
       </c>
       <c r="F30">
-        <f>IF(Q30="",1,Q30)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.5199999999999997E-2</v>
       </c>
       <c r="I30">
@@ -3436,7 +3663,7 @@
         <v>44</v>
       </c>
       <c r="N30">
-        <f>IF(RIGHT(TRIM(L30),2)="-1",B30,-B30)</f>
+        <f t="shared" si="3"/>
         <v>-2</v>
       </c>
       <c r="O30">
@@ -3446,7 +3673,7 @@
         <v>0.03</v>
       </c>
       <c r="R30">
-        <f>N30*D30*E30*F30</f>
+        <f t="shared" si="4"/>
         <v>-5.0399999999999993E-2</v>
       </c>
     </row>
@@ -3455,21 +3682,21 @@
         <v>-1</v>
       </c>
       <c r="D31">
-        <f>IF(O31="",1,O31)</f>
-        <v>0.7</v>
-      </c>
-      <c r="E31">
-        <f>IF(P31="",1,P31)</f>
-        <v>1</v>
-      </c>
-      <c r="F31">
-        <f>IF(Q31="",1,Q31)</f>
-        <v>1</v>
-      </c>
-      <c r="G31">
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="5"/>
+        <v>0.7</v>
+      </c>
       <c r="I31">
         <v>0</v>
       </c>
@@ -3486,14 +3713,14 @@
         <v>25</v>
       </c>
       <c r="N31">
-        <f>IF(RIGHT(TRIM(L31),2)="-1",B31,-B31)</f>
+        <f t="shared" si="3"/>
         <v>-1</v>
       </c>
       <c r="O31">
         <v>0.7</v>
       </c>
       <c r="R31">
-        <f>N31*D31*E31*F31</f>
+        <f t="shared" si="4"/>
         <v>-0.7</v>
       </c>
     </row>
@@ -3502,19 +3729,19 @@
         <v>-1</v>
       </c>
       <c r="D32">
-        <f>IF(O32="",1,O32)</f>
+        <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
       <c r="E32">
-        <f>IF(P32="",1,P32)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F32">
-        <f>IF(Q32="",1,Q32)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I32">
@@ -3533,7 +3760,7 @@
         <v>39</v>
       </c>
       <c r="N32">
-        <f>IF(RIGHT(TRIM(L32),2)="-1",B32,-B32)</f>
+        <f t="shared" si="3"/>
         <v>-1</v>
       </c>
       <c r="O32">
@@ -3543,7 +3770,7 @@
         <v>0</v>
       </c>
       <c r="R32">
-        <f>N32*D32*E32*F32</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3552,19 +3779,19 @@
         <v>1</v>
       </c>
       <c r="D33">
-        <f>IF(O33="",1,O33)</f>
+        <f t="shared" si="0"/>
         <v>0.89</v>
       </c>
       <c r="E33">
-        <f>IF(P33="",1,P33)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F33">
-        <f>IF(Q33="",1,Q33)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I33">
@@ -3583,7 +3810,7 @@
         <v>40</v>
       </c>
       <c r="N33">
-        <f>IF(RIGHT(TRIM(L33),2)="-1",B33,-B33)</f>
+        <f t="shared" si="3"/>
         <v>-1</v>
       </c>
       <c r="O33">
@@ -3593,7 +3820,7 @@
         <v>0</v>
       </c>
       <c r="R33">
-        <f>N33*D33*E33*F33</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3602,19 +3829,19 @@
         <v>-1</v>
       </c>
       <c r="D34">
-        <f>IF(O34="",1,O34)</f>
+        <f t="shared" si="0"/>
         <v>0.48</v>
       </c>
       <c r="E34">
-        <f>IF(P34="",1,P34)</f>
+        <f t="shared" si="1"/>
         <v>0.93</v>
       </c>
       <c r="F34">
-        <f>IF(Q34="",1,Q34)</f>
+        <f t="shared" si="2"/>
         <v>0.26</v>
       </c>
       <c r="G34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.11606400000000001</v>
       </c>
       <c r="I34">
@@ -3633,7 +3860,7 @@
         <v>41</v>
       </c>
       <c r="N34">
-        <f>IF(RIGHT(TRIM(L34),2)="-1",B34,-B34)</f>
+        <f t="shared" si="3"/>
         <v>-1</v>
       </c>
       <c r="O34">
@@ -3646,7 +3873,7 @@
         <v>0.26</v>
       </c>
       <c r="R34">
-        <f>N34*D34*E34*F34</f>
+        <f t="shared" si="4"/>
         <v>-0.11606400000000001</v>
       </c>
     </row>
@@ -3655,51 +3882,51 @@
         <v>2</v>
       </c>
       <c r="D35">
-        <f>IF(O35="",1,O35)</f>
+        <f t="shared" ref="D35:D58" si="6">IF(O35="",1,O35)</f>
         <v>0.52</v>
       </c>
       <c r="E35">
-        <f>IF(P35="",1,P35)</f>
+        <f t="shared" ref="E35:E58" si="7">IF(P35="",1,P35)</f>
         <v>0.93</v>
       </c>
       <c r="F35">
-        <f>IF(Q35="",1,Q35)</f>
+        <f t="shared" ref="F35:F58" si="8">IF(Q35="",1,Q35)</f>
         <v>0.26</v>
       </c>
       <c r="G35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.12573600000000001</v>
       </c>
-      <c r="I35" s="9">
-        <v>0</v>
-      </c>
-      <c r="J35" s="9">
-        <v>1</v>
-      </c>
-      <c r="K35" s="9">
-        <v>1</v>
-      </c>
-      <c r="L35" s="9" t="s">
+      <c r="I35" s="10">
+        <v>0</v>
+      </c>
+      <c r="J35" s="10">
+        <v>1</v>
+      </c>
+      <c r="K35" s="10">
+        <v>1</v>
+      </c>
+      <c r="L35" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="M35" s="9" t="s">
+      <c r="M35" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="N35" s="9">
-        <f>IF(RIGHT(TRIM(L35),2)="-1",B35,-B35)</f>
+      <c r="N35" s="10">
+        <f t="shared" ref="N35:N58" si="9">IF(RIGHT(TRIM(L35),2)="-1",B35,-B35)</f>
         <v>-2</v>
       </c>
-      <c r="O35" s="9">
+      <c r="O35" s="10">
         <v>0.52</v>
       </c>
-      <c r="P35" s="9">
+      <c r="P35" s="10">
         <v>0.93</v>
       </c>
-      <c r="Q35" s="9">
+      <c r="Q35" s="10">
         <v>0.26</v>
       </c>
-      <c r="R35" s="9">
-        <f>N35*D35*E35*F35</f>
+      <c r="R35" s="10">
+        <f t="shared" ref="R35:R58" si="10">N35*D35*E35*F35</f>
         <v>-0.25147200000000003</v>
       </c>
     </row>
@@ -3708,48 +3935,49 @@
         <v>-1</v>
       </c>
       <c r="D36">
-        <f>IF(O36="",1,O36)</f>
+        <f t="shared" si="6"/>
         <v>0.41</v>
       </c>
       <c r="E36">
-        <f>IF(P36="",1,P36)</f>
+        <f t="shared" si="7"/>
         <v>0.96</v>
       </c>
       <c r="F36">
-        <f>IF(Q36="",1,Q36)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.39359999999999995</v>
       </c>
-      <c r="I36">
-        <v>0</v>
-      </c>
-      <c r="J36">
-        <v>1</v>
-      </c>
-      <c r="K36">
-        <v>1</v>
-      </c>
-      <c r="L36" t="s">
+      <c r="I36" s="10">
+        <v>0</v>
+      </c>
+      <c r="J36" s="10">
+        <v>1</v>
+      </c>
+      <c r="K36" s="10">
+        <v>1</v>
+      </c>
+      <c r="L36" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="M36" t="s">
+      <c r="M36" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="N36">
-        <f>IF(RIGHT(TRIM(L36),2)="-1",B36,-B36)</f>
-        <v>-1</v>
-      </c>
-      <c r="O36">
+      <c r="N36" s="10">
+        <f t="shared" si="9"/>
+        <v>-1</v>
+      </c>
+      <c r="O36" s="10">
         <v>0.41</v>
       </c>
-      <c r="P36">
+      <c r="P36" s="10">
         <v>0.96</v>
       </c>
-      <c r="R36">
-        <f>N36*D36*E36*F36</f>
+      <c r="Q36" s="10"/>
+      <c r="R36" s="10">
+        <f t="shared" si="10"/>
         <v>-0.39359999999999995</v>
       </c>
     </row>
@@ -3758,48 +3986,49 @@
         <v>2</v>
       </c>
       <c r="D37">
-        <f>IF(O37="",1,O37)</f>
+        <f t="shared" si="6"/>
         <v>0.59</v>
       </c>
       <c r="E37">
-        <f>IF(P37="",1,P37)</f>
+        <f t="shared" si="7"/>
         <v>0.96</v>
       </c>
       <c r="F37">
-        <f>IF(Q37="",1,Q37)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.5663999999999999</v>
       </c>
-      <c r="I37">
-        <v>0</v>
-      </c>
-      <c r="J37">
-        <v>1</v>
-      </c>
-      <c r="K37">
-        <v>1</v>
-      </c>
-      <c r="L37" t="s">
+      <c r="I37" s="10">
+        <v>0</v>
+      </c>
+      <c r="J37" s="10">
+        <v>1</v>
+      </c>
+      <c r="K37" s="10">
+        <v>1</v>
+      </c>
+      <c r="L37" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="M37" t="s">
+      <c r="M37" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="N37">
-        <f>IF(RIGHT(TRIM(L37),2)="-1",B37,-B37)</f>
+      <c r="N37" s="10">
+        <f t="shared" si="9"/>
         <v>-2</v>
       </c>
-      <c r="O37">
+      <c r="O37" s="10">
         <v>0.59</v>
       </c>
-      <c r="P37">
+      <c r="P37" s="10">
         <v>0.96</v>
       </c>
-      <c r="R37">
-        <f>N37*D37*E37*F37</f>
+      <c r="Q37" s="10"/>
+      <c r="R37" s="10">
+        <f t="shared" si="10"/>
         <v>-1.1327999999999998</v>
       </c>
     </row>
@@ -3808,45 +4037,47 @@
         <v>1</v>
       </c>
       <c r="D38">
-        <f>IF(O38="",1,O38)</f>
+        <f t="shared" si="6"/>
         <v>0.04</v>
       </c>
       <c r="E38">
-        <f>IF(P38="",1,P38)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="F38">
-        <f>IF(Q38="",1,Q38)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
-      <c r="I38">
-        <v>0</v>
-      </c>
-      <c r="J38">
-        <v>1</v>
-      </c>
-      <c r="K38">
-        <v>2</v>
-      </c>
-      <c r="L38" t="s">
+      <c r="I38" s="10">
+        <v>0</v>
+      </c>
+      <c r="J38" s="10">
+        <v>1</v>
+      </c>
+      <c r="K38" s="10">
+        <v>2</v>
+      </c>
+      <c r="L38" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="M38" t="s">
+      <c r="M38" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="N38">
-        <f>IF(RIGHT(TRIM(L38),2)="-1",B38,-B38)</f>
-        <v>1</v>
-      </c>
-      <c r="O38">
+      <c r="N38" s="10">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O38" s="10">
         <v>0.04</v>
       </c>
-      <c r="R38">
-        <f>N38*D38*E38*F38</f>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="10">
+        <f t="shared" si="10"/>
         <v>0.04</v>
       </c>
     </row>
@@ -3855,19 +4086,19 @@
         <v>1</v>
       </c>
       <c r="D39">
-        <f>IF(O39="",1,O39)</f>
+        <f t="shared" si="6"/>
         <v>0.06</v>
       </c>
       <c r="E39">
-        <f>IF(P39="",1,P39)</f>
+        <f t="shared" si="7"/>
         <v>0.26</v>
       </c>
       <c r="F39">
-        <f>IF(Q39="",1,Q39)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1.5599999999999999E-2</v>
       </c>
       <c r="I39" s="10">
@@ -3886,7 +4117,7 @@
         <v>33</v>
       </c>
       <c r="N39" s="10">
-        <f>IF(RIGHT(TRIM(L39),2)="-1",B39,-B39)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="O39" s="10">
@@ -3897,7 +4128,7 @@
       </c>
       <c r="Q39" s="10"/>
       <c r="R39" s="10">
-        <f>N39*D39*E39*F39</f>
+        <f t="shared" si="10"/>
         <v>1.5599999999999999E-2</v>
       </c>
     </row>
@@ -3906,19 +4137,19 @@
         <v>-1</v>
       </c>
       <c r="D40">
-        <f>IF(O40="",1,O40)</f>
+        <f t="shared" si="6"/>
         <v>0.01</v>
       </c>
       <c r="E40">
-        <f>IF(P40="",1,P40)</f>
+        <f t="shared" si="7"/>
         <v>0.26</v>
       </c>
       <c r="F40">
-        <f>IF(Q40="",1,Q40)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.6000000000000003E-3</v>
       </c>
       <c r="I40">
@@ -3937,7 +4168,7 @@
         <v>34</v>
       </c>
       <c r="N40">
-        <f>IF(RIGHT(TRIM(L40),2)="-1",B40,-B40)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="O40">
@@ -3947,7 +4178,7 @@
         <v>0.26</v>
       </c>
       <c r="R40">
-        <f>N40*D40*E40*F40</f>
+        <f t="shared" si="10"/>
         <v>2.6000000000000003E-3</v>
       </c>
     </row>
@@ -3956,19 +4187,19 @@
         <v>1</v>
       </c>
       <c r="D41">
-        <f>IF(O41="",1,O41)</f>
+        <f t="shared" si="6"/>
         <v>0.08</v>
       </c>
       <c r="E41">
-        <f>IF(P41="",1,P41)</f>
+        <f t="shared" si="7"/>
         <v>0.09</v>
       </c>
       <c r="F41">
-        <f>IF(Q41="",1,Q41)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I41">
@@ -3987,7 +4218,7 @@
         <v>35</v>
       </c>
       <c r="N41">
-        <f>IF(RIGHT(TRIM(L41),2)="-1",B41,-B41)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="O41">
@@ -4000,7 +4231,7 @@
         <v>0</v>
       </c>
       <c r="R41">
-        <f>N41*D41*E41*F41</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -4009,19 +4240,19 @@
         <v>-2</v>
       </c>
       <c r="D42">
-        <f>IF(O42="",1,O42)</f>
+        <f t="shared" si="6"/>
         <v>0.92</v>
       </c>
       <c r="E42">
-        <f>IF(P42="",1,P42)</f>
+        <f t="shared" si="7"/>
         <v>0.09</v>
       </c>
       <c r="F42">
-        <f>IF(Q42="",1,Q42)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I42">
@@ -4040,7 +4271,7 @@
         <v>36</v>
       </c>
       <c r="N42">
-        <f>IF(RIGHT(TRIM(L42),2)="-1",B42,-B42)</f>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="O42">
@@ -4053,7 +4284,7 @@
         <v>0</v>
       </c>
       <c r="R42">
-        <f>N42*D42*E42*F42</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -4062,19 +4293,19 @@
         <v>1</v>
       </c>
       <c r="D43">
-        <f>IF(O43="",1,O43)</f>
+        <f t="shared" si="6"/>
         <v>0.09</v>
       </c>
       <c r="E43">
-        <f>IF(P43="",1,P43)</f>
+        <f t="shared" si="7"/>
         <v>0.04</v>
       </c>
       <c r="F43">
-        <f>IF(Q43="",1,Q43)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>3.5999999999999999E-3</v>
       </c>
       <c r="I43">
@@ -4093,7 +4324,7 @@
         <v>37</v>
       </c>
       <c r="N43">
-        <f>IF(RIGHT(TRIM(L43),2)="-1",B43,-B43)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="O43">
@@ -4103,7 +4334,7 @@
         <v>0.04</v>
       </c>
       <c r="R43">
-        <f>N43*D43*E43*F43</f>
+        <f t="shared" si="10"/>
         <v>3.5999999999999999E-3</v>
       </c>
     </row>
@@ -4112,19 +4343,19 @@
         <v>-2</v>
       </c>
       <c r="D44">
-        <f>IF(O44="",1,O44)</f>
+        <f t="shared" si="6"/>
         <v>0.91</v>
       </c>
       <c r="E44">
-        <f>IF(P44="",1,P44)</f>
+        <f t="shared" si="7"/>
         <v>0.04</v>
       </c>
       <c r="F44">
-        <f>IF(Q44="",1,Q44)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>3.6400000000000002E-2</v>
       </c>
       <c r="I44">
@@ -4143,7 +4374,7 @@
         <v>38</v>
       </c>
       <c r="N44">
-        <f>IF(RIGHT(TRIM(L44),2)="-1",B44,-B44)</f>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="O44">
@@ -4153,7 +4384,7 @@
         <v>0.04</v>
       </c>
       <c r="R44">
-        <f>N44*D44*E44*F44</f>
+        <f t="shared" si="10"/>
         <v>7.2800000000000004E-2</v>
       </c>
     </row>
@@ -4162,19 +4393,19 @@
         <v>-1</v>
       </c>
       <c r="D45">
-        <f>IF(O45="",1,O45)</f>
+        <f t="shared" si="6"/>
         <v>0.19</v>
       </c>
       <c r="E45">
-        <f>IF(P45="",1,P45)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="F45">
-        <f>IF(Q45="",1,Q45)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.19</v>
       </c>
       <c r="I45">
@@ -4193,14 +4424,14 @@
         <v>32</v>
       </c>
       <c r="N45">
-        <f>IF(RIGHT(TRIM(L45),2)="-1",B45,-B45)</f>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="O45">
         <v>0.19</v>
       </c>
       <c r="R45">
-        <f>N45*D45*E45*F45</f>
+        <f t="shared" si="10"/>
         <v>-0.19</v>
       </c>
     </row>
@@ -4209,19 +4440,19 @@
         <v>-1</v>
       </c>
       <c r="D46">
-        <f>IF(O46="",1,O46)</f>
+        <f t="shared" si="6"/>
         <v>0.68</v>
       </c>
       <c r="E46">
-        <f>IF(P46="",1,P46)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F46">
-        <f>IF(Q46="",1,Q46)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I46">
@@ -4240,7 +4471,7 @@
         <v>45</v>
       </c>
       <c r="N46">
-        <f>IF(RIGHT(TRIM(L46),2)="-1",B46,-B46)</f>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="O46">
@@ -4250,7 +4481,7 @@
         <v>0</v>
       </c>
       <c r="R46">
-        <f>N46*D46*E46*F46</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -4259,19 +4490,19 @@
         <v>0</v>
       </c>
       <c r="D47">
-        <f>IF(O47="",1,O47)</f>
+        <f t="shared" si="6"/>
         <v>0.08</v>
       </c>
       <c r="E47">
-        <f>IF(P47="",1,P47)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F47">
-        <f>IF(Q47="",1,Q47)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I47">
@@ -4290,7 +4521,7 @@
         <v>46</v>
       </c>
       <c r="N47">
-        <f>IF(RIGHT(TRIM(L47),2)="-1",B47,-B47)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O47">
@@ -4300,7 +4531,7 @@
         <v>0</v>
       </c>
       <c r="R47">
-        <f>N47*D47*E47*F47</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -4309,51 +4540,51 @@
         <v>-1</v>
       </c>
       <c r="D48">
-        <f>IF(O48="",1,O48)</f>
+        <f t="shared" si="6"/>
         <v>0.49</v>
       </c>
       <c r="E48">
-        <f>IF(P48="",1,P48)</f>
+        <f t="shared" si="7"/>
         <v>0.93</v>
       </c>
       <c r="F48">
-        <f>IF(Q48="",1,Q48)</f>
+        <f t="shared" si="8"/>
         <v>0.78</v>
       </c>
       <c r="G48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.35544599999999998</v>
       </c>
-      <c r="I48" s="11">
-        <v>1</v>
-      </c>
-      <c r="J48" s="11">
-        <v>1</v>
-      </c>
-      <c r="K48" s="11">
-        <v>1</v>
-      </c>
-      <c r="L48" s="11" t="s">
+      <c r="I48" s="10">
+        <v>1</v>
+      </c>
+      <c r="J48" s="10">
+        <v>1</v>
+      </c>
+      <c r="K48" s="10">
+        <v>1</v>
+      </c>
+      <c r="L48" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="M48" s="11" t="s">
+      <c r="M48" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="N48" s="11">
-        <f>IF(RIGHT(TRIM(L48),2)="-1",B48,-B48)</f>
-        <v>-1</v>
-      </c>
-      <c r="O48" s="11">
+      <c r="N48" s="10">
+        <f t="shared" si="9"/>
+        <v>-1</v>
+      </c>
+      <c r="O48" s="10">
         <v>0.49</v>
       </c>
-      <c r="P48" s="11">
+      <c r="P48" s="10">
         <v>0.93</v>
       </c>
-      <c r="Q48" s="11">
+      <c r="Q48" s="10">
         <v>0.78</v>
       </c>
-      <c r="R48" s="11">
-        <f>N48*D48*E48*F48</f>
+      <c r="R48" s="10">
+        <f t="shared" si="10"/>
         <v>-0.35544599999999998</v>
       </c>
     </row>
@@ -4362,19 +4593,19 @@
         <v>0</v>
       </c>
       <c r="D49">
-        <f>IF(O49="",1,O49)</f>
+        <f t="shared" si="6"/>
         <v>0.51</v>
       </c>
       <c r="E49">
-        <f>IF(P49="",1,P49)</f>
+        <f t="shared" si="7"/>
         <v>0.93</v>
       </c>
       <c r="F49">
-        <f>IF(Q49="",1,Q49)</f>
+        <f t="shared" si="8"/>
         <v>0.78</v>
       </c>
       <c r="G49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.36995400000000006</v>
       </c>
       <c r="I49">
@@ -4393,7 +4624,7 @@
         <v>48</v>
       </c>
       <c r="N49">
-        <f>IF(RIGHT(TRIM(L49),2)="-1",B49,-B49)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O49">
@@ -4406,7 +4637,7 @@
         <v>0.78</v>
       </c>
       <c r="R49">
-        <f>N49*D49*E49*F49</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -4415,19 +4646,19 @@
         <v>-1</v>
       </c>
       <c r="D50">
-        <f>IF(O50="",1,O50)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E50">
-        <f>IF(P50="",1,P50)</f>
+        <f t="shared" si="7"/>
         <v>0.96</v>
       </c>
       <c r="F50">
-        <f>IF(Q50="",1,Q50)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I50">
@@ -4446,7 +4677,7 @@
         <v>49</v>
       </c>
       <c r="N50">
-        <f>IF(RIGHT(TRIM(L50),2)="-1",B50,-B50)</f>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="O50">
@@ -4456,7 +4687,7 @@
         <v>0.96</v>
       </c>
       <c r="R50">
-        <f>N50*D50*E50*F50</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -4465,19 +4696,19 @@
         <v>0</v>
       </c>
       <c r="D51">
-        <f>IF(O51="",1,O51)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="E51">
-        <f>IF(P51="",1,P51)</f>
+        <f t="shared" si="7"/>
         <v>0.96</v>
       </c>
       <c r="F51">
-        <f>IF(Q51="",1,Q51)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.96</v>
       </c>
       <c r="I51">
@@ -4496,7 +4727,7 @@
         <v>50</v>
       </c>
       <c r="N51">
-        <f>IF(RIGHT(TRIM(L51),2)="-1",B51,-B51)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O51">
@@ -4506,7 +4737,7 @@
         <v>0.96</v>
       </c>
       <c r="R51">
-        <f>N51*D51*E51*F51</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -4515,19 +4746,19 @@
         <v>1</v>
       </c>
       <c r="D52">
-        <f>IF(O52="",1,O52)</f>
+        <f t="shared" si="6"/>
         <v>0.04</v>
       </c>
       <c r="E52">
-        <f>IF(P52="",1,P52)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="F52">
-        <f>IF(Q52="",1,Q52)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="I52">
@@ -4546,14 +4777,14 @@
         <v>32</v>
       </c>
       <c r="N52">
-        <f>IF(RIGHT(TRIM(L52),2)="-1",B52,-B52)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="O52">
         <v>0.04</v>
       </c>
       <c r="R52">
-        <f>N52*D52*E52*F52</f>
+        <f t="shared" si="10"/>
         <v>0.04</v>
       </c>
     </row>
@@ -4562,19 +4793,19 @@
         <v>1</v>
       </c>
       <c r="D53">
-        <f>IF(O53="",1,O53)</f>
+        <f t="shared" si="6"/>
         <v>0.06</v>
       </c>
       <c r="E53">
-        <f>IF(P53="",1,P53)</f>
+        <f t="shared" si="7"/>
         <v>0.78</v>
       </c>
       <c r="F53">
-        <f>IF(Q53="",1,Q53)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>4.6800000000000001E-2</v>
       </c>
       <c r="I53">
@@ -4593,7 +4824,7 @@
         <v>45</v>
       </c>
       <c r="N53">
-        <f>IF(RIGHT(TRIM(L53),2)="-1",B53,-B53)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="O53">
@@ -4603,7 +4834,7 @@
         <v>0.78</v>
       </c>
       <c r="R53">
-        <f>N53*D53*E53*F53</f>
+        <f t="shared" si="10"/>
         <v>4.6800000000000001E-2</v>
       </c>
     </row>
@@ -4612,19 +4843,19 @@
         <v>0</v>
       </c>
       <c r="D54">
-        <f>IF(O54="",1,O54)</f>
+        <f t="shared" si="6"/>
         <v>0.01</v>
       </c>
       <c r="E54">
-        <f>IF(P54="",1,P54)</f>
+        <f t="shared" si="7"/>
         <v>0.78</v>
       </c>
       <c r="F54">
-        <f>IF(Q54="",1,Q54)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.8000000000000005E-3</v>
       </c>
       <c r="I54">
@@ -4643,7 +4874,7 @@
         <v>46</v>
       </c>
       <c r="N54">
-        <f>IF(RIGHT(TRIM(L54),2)="-1",B54,-B54)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O54">
@@ -4653,7 +4884,7 @@
         <v>0.78</v>
       </c>
       <c r="R54">
-        <f>N54*D54*E54*F54</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -4662,51 +4893,51 @@
         <v>1</v>
       </c>
       <c r="D55">
-        <f>IF(O55="",1,O55)</f>
+        <f t="shared" si="6"/>
         <v>0.08</v>
       </c>
       <c r="E55">
-        <f>IF(P55="",1,P55)</f>
+        <f t="shared" si="7"/>
         <v>0.24</v>
       </c>
       <c r="F55">
-        <f>IF(Q55="",1,Q55)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G55">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I55" s="11">
-        <v>1</v>
-      </c>
-      <c r="J55" s="11">
-        <v>1</v>
-      </c>
-      <c r="K55" s="11">
-        <v>2</v>
-      </c>
-      <c r="L55" s="11" t="s">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I55" s="10">
+        <v>1</v>
+      </c>
+      <c r="J55" s="10">
+        <v>1</v>
+      </c>
+      <c r="K55" s="10">
+        <v>2</v>
+      </c>
+      <c r="L55" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="M55" s="11" t="s">
+      <c r="M55" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="N55" s="11">
-        <f>IF(RIGHT(TRIM(L55),2)="-1",B55,-B55)</f>
-        <v>1</v>
-      </c>
-      <c r="O55" s="11">
+      <c r="N55" s="10">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O55" s="10">
         <v>0.08</v>
       </c>
-      <c r="P55" s="11">
+      <c r="P55" s="10">
         <v>0.24</v>
       </c>
-      <c r="Q55" s="11">
-        <v>0</v>
-      </c>
-      <c r="R55" s="11">
-        <f>N55*D55*E55*F55</f>
+      <c r="Q55" s="10">
+        <v>0</v>
+      </c>
+      <c r="R55" s="10">
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -4715,19 +4946,19 @@
         <v>0</v>
       </c>
       <c r="D56">
-        <f>IF(O56="",1,O56)</f>
+        <f t="shared" si="6"/>
         <v>0.92</v>
       </c>
       <c r="E56">
-        <f>IF(P56="",1,P56)</f>
+        <f t="shared" si="7"/>
         <v>0.24</v>
       </c>
       <c r="F56">
-        <f>IF(Q56="",1,Q56)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I56">
@@ -4746,7 +4977,7 @@
         <v>48</v>
       </c>
       <c r="N56">
-        <f>IF(RIGHT(TRIM(L56),2)="-1",B56,-B56)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O56">
@@ -4759,7 +4990,7 @@
         <v>0</v>
       </c>
       <c r="R56">
-        <f>N56*D56*E56*F56</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -4768,19 +4999,19 @@
         <v>1</v>
       </c>
       <c r="D57">
-        <f>IF(O57="",1,O57)</f>
+        <f t="shared" si="6"/>
         <v>0.09</v>
       </c>
       <c r="E57">
-        <f>IF(P57="",1,P57)</f>
+        <f t="shared" si="7"/>
         <v>0.03</v>
       </c>
       <c r="F57">
-        <f>IF(Q57="",1,Q57)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.6999999999999997E-3</v>
       </c>
       <c r="I57">
@@ -4799,7 +5030,7 @@
         <v>49</v>
       </c>
       <c r="N57">
-        <f>IF(RIGHT(TRIM(L57),2)="-1",B57,-B57)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="O57">
@@ -4809,7 +5040,7 @@
         <v>0.03</v>
       </c>
       <c r="R57">
-        <f>N57*D57*E57*F57</f>
+        <f t="shared" si="10"/>
         <v>2.6999999999999997E-3</v>
       </c>
     </row>
@@ -4818,19 +5049,19 @@
         <v>0</v>
       </c>
       <c r="D58">
-        <f>IF(O58="",1,O58)</f>
+        <f t="shared" si="6"/>
         <v>0.91</v>
       </c>
       <c r="E58">
-        <f>IF(P58="",1,P58)</f>
+        <f t="shared" si="7"/>
         <v>0.03</v>
       </c>
       <c r="F58">
-        <f>IF(Q58="",1,Q58)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.7300000000000001E-2</v>
       </c>
       <c r="I58">
@@ -4849,7 +5080,7 @@
         <v>50</v>
       </c>
       <c r="N58">
-        <f>IF(RIGHT(TRIM(L58),2)="-1",B58,-B58)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O58">
@@ -4859,7 +5090,7 @@
         <v>0.03</v>
       </c>
       <c r="R58">
-        <f>N58*D58*E58*F58</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -4876,121 +5107,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2">
-        <v>0.2044</v>
-      </c>
-      <c r="C2">
-        <v>0.2303</v>
-      </c>
-      <c r="D2">
-        <v>0.56520000000000004</v>
-      </c>
-      <c r="E2">
-        <v>0.90200000000000002</v>
-      </c>
-      <c r="F2">
-        <v>7.5899999999999995E-2</v>
-      </c>
-      <c r="G2">
-        <v>2.2100000000000002E-2</v>
-      </c>
-      <c r="H2">
-        <v>0.85140000000000005</v>
-      </c>
-      <c r="I2">
-        <v>0.14860000000000001</v>
-      </c>
-      <c r="J2">
-        <v>8.0000000000000004E-4</v>
-      </c>
-      <c r="K2">
-        <v>0.99919999999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>0.2913</v>
-      </c>
-      <c r="C3">
-        <v>0.55379999999999996</v>
-      </c>
-      <c r="D3">
-        <v>0.15490000000000001</v>
-      </c>
-      <c r="E3">
-        <v>0.69530000000000003</v>
-      </c>
-      <c r="F3">
-        <v>0.1981</v>
-      </c>
-      <c r="G3">
-        <v>0.1065</v>
-      </c>
-      <c r="H3">
-        <v>0.63839999999999997</v>
-      </c>
-      <c r="I3">
-        <v>0.36159999999999998</v>
-      </c>
-      <c r="J3">
-        <v>0.61970000000000003</v>
-      </c>
-      <c r="K3">
-        <v>0.38030000000000003</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <f>B2+C2+D2</f>
-        <v>0.99990000000000001</v>
-      </c>
-      <c r="E6">
-        <f>E2+F2+G2</f>
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <f>H2+I2</f>
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <f>J2+K2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <f>B3+C3+D3</f>
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <f>E3+F3+G3</f>
-        <v>0.99990000000000001</v>
-      </c>
-      <c r="H7">
-        <f>H3+I3</f>
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <f>J3+K3</f>
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="B1:M121"/>
@@ -9306,4 +9422,1652 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:AJ58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="8" width="11.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>-1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>-1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" t="s">
+        <v>59</v>
+      </c>
+      <c r="V4">
+        <v>1</v>
+      </c>
+      <c r="W4" t="s">
+        <v>106</v>
+      </c>
+      <c r="AJ4" t="str">
+        <f>"//"&amp;V4&amp;" "&amp;W4</f>
+        <v>//1 Fill A braincells with -1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" t="s">
+        <v>60</v>
+      </c>
+      <c r="V5">
+        <v>2</v>
+      </c>
+      <c r="W5" t="s">
+        <v>101</v>
+      </c>
+      <c r="AJ5" t="str">
+        <f t="shared" ref="AJ5:AJ13" si="0">"//"&amp;V5&amp;" "&amp;W5</f>
+        <v>//2 Make Coins2 = Coins</v>
+      </c>
+    </row>
+    <row r="6" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="14">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="14">
+        <v>-1</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="V6">
+        <v>3</v>
+      </c>
+      <c r="W6" t="s">
+        <v>103</v>
+      </c>
+      <c r="AJ6" t="str">
+        <f t="shared" si="0"/>
+        <v>//3 Filter longest (n length) paths where A ends</v>
+      </c>
+    </row>
+    <row r="7" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" s="14">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="14">
+        <v>0</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="V7">
+        <v>4</v>
+      </c>
+      <c r="W7" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ7" t="str">
+        <f t="shared" si="0"/>
+        <v>//4 Scan groups of moves (A6, Ap……A16, A17)</v>
+      </c>
+    </row>
+    <row r="8" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>-1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" t="s">
+        <v>63</v>
+      </c>
+      <c r="V8">
+        <v>5</v>
+      </c>
+      <c r="W8" t="s">
+        <v>102</v>
+      </c>
+      <c r="AJ8" t="str">
+        <f t="shared" si="0"/>
+        <v>//5 Calculate sum of (multiplication of all P probabilites * coins2 in the same row) for each A in a group</v>
+      </c>
+    </row>
+    <row r="9" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" t="s">
+        <v>64</v>
+      </c>
+      <c r="V9">
+        <v>6</v>
+      </c>
+      <c r="W9" t="s">
+        <v>109</v>
+      </c>
+      <c r="AJ9" t="str">
+        <f t="shared" si="0"/>
+        <v>//6 Choose the best outcome, fill its A with 1, and replace all other A with 0 in the group (verify if A was -1 before replacement, otherwise - exception)</v>
+      </c>
+    </row>
+    <row r="10" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>80</v>
+      </c>
+      <c r="O10" s="14">
+        <v>1</v>
+      </c>
+      <c r="P10" s="14">
+        <v>-1</v>
+      </c>
+      <c r="Q10" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="R10" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="V10">
+        <v>7</v>
+      </c>
+      <c r="W10" t="s">
+        <v>104</v>
+      </c>
+      <c r="AJ10" t="str">
+        <f t="shared" si="0"/>
+        <v>//7 If N&gt;2, replace coins2 with coins2 * A(n) * p(n-1); delete A(n) and p(n-1)</v>
+      </c>
+    </row>
+    <row r="11" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" t="s">
+        <v>81</v>
+      </c>
+      <c r="J11" s="14">
+        <v>1</v>
+      </c>
+      <c r="K11" s="14">
+        <v>-1</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="M11" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="O11" s="13">
+        <v>2</v>
+      </c>
+      <c r="P11" s="13">
+        <v>-1</v>
+      </c>
+      <c r="Q11" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="R11" s="12"/>
+      <c r="V11">
+        <v>8</v>
+      </c>
+      <c r="W11" t="s">
+        <v>105</v>
+      </c>
+      <c r="AJ11" t="str">
+        <f t="shared" si="0"/>
+        <v>//8 While N&gt;1, continue step 3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" t="s">
+        <v>82</v>
+      </c>
+      <c r="J12" s="14">
+        <v>1</v>
+      </c>
+      <c r="K12" s="14">
+        <v>0</v>
+      </c>
+      <c r="L12" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="V12">
+        <v>9</v>
+      </c>
+      <c r="W12" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ12" t="str">
+        <f t="shared" si="0"/>
+        <v>//9 Verify if any -1 brain cell is left in A</v>
+      </c>
+    </row>
+    <row r="13" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G13" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13" t="s">
+        <v>83</v>
+      </c>
+      <c r="J13" s="13">
+        <v>2</v>
+      </c>
+      <c r="K13" s="13">
+        <v>-1</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="M13" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="V13">
+        <v>10</v>
+      </c>
+      <c r="W13" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ13" t="str">
+        <f t="shared" si="0"/>
+        <v>//10 Make a copy of A, run normalise, verify if anything is changed</v>
+      </c>
+    </row>
+    <row r="14" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G14" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" t="s">
+        <v>84</v>
+      </c>
+      <c r="J14" s="13">
+        <v>2</v>
+      </c>
+      <c r="K14" s="13">
+        <v>-2</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="O14" s="14">
+        <v>1</v>
+      </c>
+      <c r="P14" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="R14" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" t="s">
+        <v>85</v>
+      </c>
+      <c r="O15" s="13">
+        <v>2</v>
+      </c>
+      <c r="P15" s="13">
+        <v>-2</v>
+      </c>
+      <c r="Q15" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="R15" s="12"/>
+    </row>
+    <row r="16" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>-1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>-1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>-1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>87</v>
+      </c>
+      <c r="G19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>17</v>
+      </c>
+      <c r="C20" s="13">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" s="13">
+        <v>-1</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>18</v>
+      </c>
+      <c r="C21" s="13">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="13">
+        <v>-2</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>19</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>-1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>89</v>
+      </c>
+      <c r="G22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>-2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>89</v>
+      </c>
+      <c r="G23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>21</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>22</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>55</v>
+      </c>
+      <c r="G25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>23</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>-1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>55</v>
+      </c>
+      <c r="G26" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>24</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
+        <v>87</v>
+      </c>
+      <c r="G27" t="s">
+        <v>56</v>
+      </c>
+      <c r="H27" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>25</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>-2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>87</v>
+      </c>
+      <c r="G28" t="s">
+        <v>56</v>
+      </c>
+      <c r="H28" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>26</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
+        <v>57</v>
+      </c>
+      <c r="G29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>27</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>-2</v>
+      </c>
+      <c r="F30" t="s">
+        <v>57</v>
+      </c>
+      <c r="G30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>28</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <v>-1</v>
+      </c>
+      <c r="F31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>29</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <v>-1</v>
+      </c>
+      <c r="F32" t="s">
+        <v>77</v>
+      </c>
+      <c r="G32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>30</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
+        <v>77</v>
+      </c>
+      <c r="G33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>31</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>-1</v>
+      </c>
+      <c r="F34" t="s">
+        <v>65</v>
+      </c>
+      <c r="G34" t="s">
+        <v>78</v>
+      </c>
+      <c r="H34" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>32</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="F35" t="s">
+        <v>65</v>
+      </c>
+      <c r="G35" t="s">
+        <v>78</v>
+      </c>
+      <c r="H35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>33</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36">
+        <v>-1</v>
+      </c>
+      <c r="F36" t="s">
+        <v>79</v>
+      </c>
+      <c r="G36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>34</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37" t="s">
+        <v>79</v>
+      </c>
+      <c r="G37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>35</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>36</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39" t="s">
+        <v>65</v>
+      </c>
+      <c r="G39" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>37</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40" t="s">
+        <v>65</v>
+      </c>
+      <c r="G40" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>38</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41" t="s">
+        <v>77</v>
+      </c>
+      <c r="G41" t="s">
+        <v>66</v>
+      </c>
+      <c r="H41" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>39</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42" t="s">
+        <v>77</v>
+      </c>
+      <c r="G42" t="s">
+        <v>66</v>
+      </c>
+      <c r="H42" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>40</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43" t="s">
+        <v>67</v>
+      </c>
+      <c r="G43" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>41</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="F44" t="s">
+        <v>67</v>
+      </c>
+      <c r="G44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>42</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="E45">
+        <v>-1</v>
+      </c>
+      <c r="F45" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>43</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46">
+        <v>-1</v>
+      </c>
+      <c r="F46" t="s">
+        <v>87</v>
+      </c>
+      <c r="G46" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>44</v>
+      </c>
+      <c r="C47">
+        <v>2</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47" t="s">
+        <v>87</v>
+      </c>
+      <c r="G47" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>45</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48">
+        <v>-1</v>
+      </c>
+      <c r="F48" t="s">
+        <v>65</v>
+      </c>
+      <c r="G48" t="s">
+        <v>88</v>
+      </c>
+      <c r="H48" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>46</v>
+      </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49" t="s">
+        <v>65</v>
+      </c>
+      <c r="G49" t="s">
+        <v>88</v>
+      </c>
+      <c r="H49" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>47</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
+      </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="E50">
+        <v>-1</v>
+      </c>
+      <c r="F50" t="s">
+        <v>89</v>
+      </c>
+      <c r="G50" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>48</v>
+      </c>
+      <c r="C51">
+        <v>2</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51" t="s">
+        <v>89</v>
+      </c>
+      <c r="G51" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>49</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>50</v>
+      </c>
+      <c r="C53">
+        <v>2</v>
+      </c>
+      <c r="D53">
+        <v>2</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53" t="s">
+        <v>65</v>
+      </c>
+      <c r="G53" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>51</v>
+      </c>
+      <c r="C54">
+        <v>2</v>
+      </c>
+      <c r="D54">
+        <v>2</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54" t="s">
+        <v>65</v>
+      </c>
+      <c r="G54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>52</v>
+      </c>
+      <c r="C55">
+        <v>2</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55" t="s">
+        <v>87</v>
+      </c>
+      <c r="G55" t="s">
+        <v>66</v>
+      </c>
+      <c r="H55" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>53</v>
+      </c>
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="D56">
+        <v>2</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56" t="s">
+        <v>87</v>
+      </c>
+      <c r="G56" t="s">
+        <v>66</v>
+      </c>
+      <c r="H56" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>54</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57" t="s">
+        <v>67</v>
+      </c>
+      <c r="G57" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>55</v>
+      </c>
+      <c r="C58">
+        <v>2</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58" t="s">
+        <v>67</v>
+      </c>
+      <c r="G58" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:V5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B2" s="15"/>
+      <c r="C2" s="16">
+        <v>0</v>
+      </c>
+      <c r="D2" s="16">
+        <v>1</v>
+      </c>
+      <c r="E2" s="16">
+        <v>2</v>
+      </c>
+      <c r="F2" s="16">
+        <v>3</v>
+      </c>
+      <c r="G2" s="16">
+        <v>4</v>
+      </c>
+      <c r="H2" s="16">
+        <v>5</v>
+      </c>
+      <c r="I2" s="16">
+        <v>6</v>
+      </c>
+      <c r="J2" s="16">
+        <v>7</v>
+      </c>
+      <c r="K2" s="16">
+        <v>8</v>
+      </c>
+      <c r="L2" s="16">
+        <v>9</v>
+      </c>
+      <c r="M2" s="16">
+        <v>10</v>
+      </c>
+      <c r="N2" s="16">
+        <v>11</v>
+      </c>
+      <c r="O2" s="16">
+        <v>12</v>
+      </c>
+      <c r="P2" s="16">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="16">
+        <v>14</v>
+      </c>
+      <c r="R2" s="16">
+        <v>15</v>
+      </c>
+      <c r="S2" s="16">
+        <v>16</v>
+      </c>
+      <c r="T2" s="16">
+        <v>17</v>
+      </c>
+      <c r="U2" s="16">
+        <v>18</v>
+      </c>
+      <c r="V2" s="16">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B3" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="15">
+        <v>0</v>
+      </c>
+      <c r="D3" s="15">
+        <v>0</v>
+      </c>
+      <c r="E3" s="15">
+        <v>1</v>
+      </c>
+      <c r="F3" s="15">
+        <v>0</v>
+      </c>
+      <c r="G3" s="15">
+        <v>0</v>
+      </c>
+      <c r="H3" s="15">
+        <v>1</v>
+      </c>
+      <c r="I3" s="15">
+        <v>1</v>
+      </c>
+      <c r="J3" s="15">
+        <v>0</v>
+      </c>
+      <c r="K3" s="15">
+        <v>0</v>
+      </c>
+      <c r="L3" s="15">
+        <v>1</v>
+      </c>
+      <c r="M3" s="15">
+        <v>0</v>
+      </c>
+      <c r="N3" s="15">
+        <v>1</v>
+      </c>
+      <c r="O3" s="15">
+        <v>0</v>
+      </c>
+      <c r="P3" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="15">
+        <v>1</v>
+      </c>
+      <c r="R3" s="15">
+        <v>0</v>
+      </c>
+      <c r="S3" s="15">
+        <v>0</v>
+      </c>
+      <c r="T3" s="15">
+        <v>1</v>
+      </c>
+      <c r="U3" s="15">
+        <v>0</v>
+      </c>
+      <c r="V3" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" s="15">
+        <v>0</v>
+      </c>
+      <c r="D4" s="15">
+        <v>1</v>
+      </c>
+      <c r="E4" s="15">
+        <v>0</v>
+      </c>
+      <c r="F4" s="15">
+        <v>0</v>
+      </c>
+      <c r="G4" s="15">
+        <v>0</v>
+      </c>
+      <c r="H4" s="15">
+        <v>1</v>
+      </c>
+      <c r="I4" s="15">
+        <v>1</v>
+      </c>
+      <c r="J4" s="15">
+        <v>0</v>
+      </c>
+      <c r="K4" s="15">
+        <v>0</v>
+      </c>
+      <c r="L4" s="15">
+        <v>1</v>
+      </c>
+      <c r="M4" s="15">
+        <v>0</v>
+      </c>
+      <c r="N4" s="15">
+        <v>1</v>
+      </c>
+      <c r="O4" s="15">
+        <v>0</v>
+      </c>
+      <c r="P4" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="15">
+        <v>0</v>
+      </c>
+      <c r="R4" s="15">
+        <v>1</v>
+      </c>
+      <c r="S4" s="15">
+        <v>0</v>
+      </c>
+      <c r="T4" s="15">
+        <v>1</v>
+      </c>
+      <c r="U4" s="15">
+        <v>0</v>
+      </c>
+      <c r="V4" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="15">
+        <v>1.04E-2</v>
+      </c>
+      <c r="D5" s="15">
+        <v>0.95720000000000005</v>
+      </c>
+      <c r="E5" s="15">
+        <v>3.2399999999999998E-2</v>
+      </c>
+      <c r="F5" s="15">
+        <v>0.33660000000000001</v>
+      </c>
+      <c r="G5" s="15">
+        <v>5.3699999999999998E-2</v>
+      </c>
+      <c r="H5" s="15">
+        <v>0.60970000000000002</v>
+      </c>
+      <c r="I5" s="15">
+        <v>0.53290000000000004</v>
+      </c>
+      <c r="J5" s="15">
+        <v>0.46710000000000002</v>
+      </c>
+      <c r="K5" s="15">
+        <v>0.15870000000000001</v>
+      </c>
+      <c r="L5" s="15">
+        <v>0.84130000000000005</v>
+      </c>
+      <c r="M5" s="15">
+        <v>1.3599999999999999E-2</v>
+      </c>
+      <c r="N5" s="15">
+        <v>0.68410000000000004</v>
+      </c>
+      <c r="O5" s="15">
+        <v>0.30230000000000001</v>
+      </c>
+      <c r="P5" s="15">
+        <v>1.49E-2</v>
+      </c>
+      <c r="Q5" s="15">
+        <v>0.1045</v>
+      </c>
+      <c r="R5" s="15">
+        <v>0.88060000000000005</v>
+      </c>
+      <c r="S5" s="15">
+        <v>0.44829999999999998</v>
+      </c>
+      <c r="T5" s="15">
+        <v>0.55169999999999997</v>
+      </c>
+      <c r="U5" s="15">
+        <v>0.70569999999999999</v>
+      </c>
+      <c r="V5" s="15">
+        <v>0.29430000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>